<commit_message>
add empty page check
</commit_message>
<xml_diff>
--- a/tucson/tucson.xlsx
+++ b/tucson/tucson.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G614"/>
+  <dimension ref="A1:G616"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19214,6 +19214,60 @@
         </is>
       </c>
     </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>Tucson</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>alberdi</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>ALBERDI PORC.60X60 DOMO NATURAL 1RA</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr">
+        <is>
+          <t>6.575 M²</t>
+        </is>
+      </c>
+      <c r="F615" t="inlineStr">
+        <is>
+          <t>https://tienda.tucsonsa.com/productos/alberdi-porc-60x60-domo-natural-1ra/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>Tucson</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>alberdi</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>ALBERDI PORC.60X60 DOMO NATURAL 1RA</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr">
+        <is>
+          <t>6.575 M²</t>
+        </is>
+      </c>
+      <c r="F616" t="inlineStr">
+        <is>
+          <t>https://tienda.tucsonsa.com/productos/alberdi-porc-60x60-domo-natural-1ra/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>